<commit_message>
Ajustes BD servicos e produtos
</commit_message>
<xml_diff>
--- a/Front-End/public/ImportSheet/modelo-produto.xlsx
+++ b/Front-End/public/ImportSheet/modelo-produto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSICOLOGIA\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B13C6E-F878-4641-B95B-2CF176B05B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D00CB68-C68E-4FBF-BEDF-3FD6F22BAC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,29 +21,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="189">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>manufacturer</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
   <si>
     <t>category</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>sku</t>
   </si>
   <si>
     <t>unitType</t>
   </si>
   <si>
-    <t>unitPrice</t>
-  </si>
-  <si>
     <t>ncm</t>
   </si>
   <si>
@@ -59,18 +47,9 @@
     <t>productOrigin</t>
   </si>
   <si>
-    <t>MTX</t>
-  </si>
-  <si>
     <t>Construção</t>
   </si>
   <si>
-    <t>Martelo de Unha Magnético – Cabeça de Aço 27 mm, Cabo de Fibra de Vidro Antiderrapante, 450 g</t>
-  </si>
-  <si>
-    <t>Martelo 27mm</t>
-  </si>
-  <si>
     <t>Unidade</t>
   </si>
   <si>
@@ -587,7 +566,25 @@
     <t>8 – Nacional – Mercadoria ou bem com Conteúdo de Importação superior a 70%</t>
   </si>
   <si>
-    <t>8205.20.00</t>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>fabricante</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>unidade_de_medida</t>
+  </si>
+  <si>
+    <t>preco_unitario</t>
+  </si>
+  <si>
+    <t>origem_do_produto</t>
   </si>
 </sst>
 </file>
@@ -1223,7 +1220,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L301"/>
+  <dimension ref="A1:L300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1237,89 +1234,67 @@
     <col min="3" max="3" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>181</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="L1" s="6" t="s">
-        <v>11</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="15" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="9">
-        <v>299</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="11">
-        <v>27.9</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="I2" s="9">
-        <v>5102</v>
-      </c>
-      <c r="J2" s="12">
-        <v>0.18</v>
-      </c>
-      <c r="K2" s="13">
-        <v>9.6500000000000002E-2</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>179</v>
-      </c>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:12" s="15" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
@@ -5479,33 +5454,19 @@
       <c r="K299" s="21"/>
       <c r="L299" s="22"/>
     </row>
-    <row r="300" spans="1:12" s="15" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A300" s="16"/>
-      <c r="B300" s="17"/>
-      <c r="C300" s="17"/>
-      <c r="D300" s="17"/>
-      <c r="E300" s="17"/>
-      <c r="F300" s="18"/>
-      <c r="G300" s="19"/>
-      <c r="H300" s="17"/>
-      <c r="I300" s="17"/>
-      <c r="J300" s="20"/>
-      <c r="K300" s="21"/>
-      <c r="L300" s="22"/>
-    </row>
-    <row r="301" spans="1:12" s="15" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A301" s="23"/>
-      <c r="B301" s="24"/>
-      <c r="C301" s="24"/>
-      <c r="D301" s="24"/>
-      <c r="E301" s="24"/>
-      <c r="F301" s="25"/>
-      <c r="G301" s="26"/>
-      <c r="H301" s="24"/>
-      <c r="I301" s="24"/>
-      <c r="J301" s="27"/>
-      <c r="K301" s="28"/>
-      <c r="L301" s="29"/>
+    <row r="300" spans="1:12" s="15" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A300" s="23"/>
+      <c r="B300" s="24"/>
+      <c r="C300" s="24"/>
+      <c r="D300" s="24"/>
+      <c r="E300" s="24"/>
+      <c r="F300" s="25"/>
+      <c r="G300" s="26"/>
+      <c r="H300" s="24"/>
+      <c r="I300" s="24"/>
+      <c r="J300" s="27"/>
+      <c r="K300" s="28"/>
+      <c r="L300" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5516,19 +5477,19 @@
           <x14:formula1>
             <xm:f>Dados!$B$2:$B$41</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F300</xm:sqref>
+          <xm:sqref>F2:F299</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3494D52-8847-47B1-9D94-B04791481045}">
           <x14:formula1>
             <xm:f>Dados!$C$2:$C$10</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L300</xm:sqref>
+          <xm:sqref>L2:L299</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C5C384C0-3C3C-4880-B7AC-D2443A71C852}">
           <x14:formula1>
             <xm:f>Dados!$A$2:$A$125</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C300</xm:sqref>
+          <xm:sqref>C2:C299</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5553,780 +5514,780 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>